<commit_message>
updates done 2:11pm 03-02-2026
</commit_message>
<xml_diff>
--- a/Excel Output/CruiseDetails.xlsx
+++ b/Excel Output/CruiseDetails.xlsx
@@ -23,13 +23,13 @@
     <t>Cruise ID</t>
   </si>
   <si>
-    <t>1,266</t>
+    <t>Renovated:2024</t>
   </si>
   <si>
     <t>2024</t>
   </si>
   <si>
-    <t>160581</t>
+    <t>123873</t>
   </si>
 </sst>
 </file>

</xml_diff>